<commit_message>
Creating py files and folder structure
</commit_message>
<xml_diff>
--- a/data/elections_results_by_department.xlsx
+++ b/data/elections_results_by_department.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidlupau/kDrive/_IU/_Modules/4th semester/22. Explorative Data Analysis and Visualization/Code/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidlupau/kDrive/_IU/_Modules/4th semester/22. Explorative Data Analysis and Visualization/visualisation_french_elections_results/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29CFE553-C10B-CD4F-B5C1-2EE0DEA29EBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA3CC31F-4EFC-934F-94FD-501E231DF37F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16480" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38400" yWindow="-3100" windowWidth="38400" windowHeight="21100" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="results" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4359" uniqueCount="422">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4359" uniqueCount="427">
   <si>
     <t>01</t>
   </si>
@@ -1302,6 +1302,21 @@
   </si>
   <si>
     <t>candidate_12_gender</t>
+  </si>
+  <si>
+    <t>candidate_3_votes_pct_voters</t>
+  </si>
+  <si>
+    <t>candidate_5_votes_pct_reg</t>
+  </si>
+  <si>
+    <t>candidate_7_votes</t>
+  </si>
+  <si>
+    <t>candidate_9_surname</t>
+  </si>
+  <si>
+    <t>candidate_11_first_name</t>
   </si>
 </sst>
 </file>
@@ -1674,8 +1689,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CK108"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="BW10" sqref="BW10"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1819,10 +1834,10 @@
         <v>355</v>
       </c>
       <c r="S1" t="s">
+        <v>356</v>
+      </c>
+      <c r="T1" t="s">
         <v>357</v>
-      </c>
-      <c r="T1" t="s">
-        <v>356</v>
       </c>
       <c r="U1" t="s">
         <v>358</v>
@@ -1837,10 +1852,10 @@
         <v>361</v>
       </c>
       <c r="Y1" t="s">
+        <v>363</v>
+      </c>
+      <c r="Z1" t="s">
         <v>362</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>363</v>
       </c>
       <c r="AA1" t="s">
         <v>364</v>
@@ -1855,181 +1870,181 @@
         <v>367</v>
       </c>
       <c r="AE1" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="AF1" t="s">
         <v>368</v>
       </c>
       <c r="AG1" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="AH1" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="AI1" t="s">
-        <v>371</v>
+        <v>422</v>
       </c>
       <c r="AJ1" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="AK1" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="AL1" t="s">
         <v>374</v>
       </c>
       <c r="AM1" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="AN1" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="AO1" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="AP1" t="s">
+        <v>379</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>381</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>380</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>382</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>423</v>
+      </c>
+      <c r="AU1" t="s">
         <v>378</v>
       </c>
-      <c r="AQ1" t="s">
-        <v>379</v>
-      </c>
-      <c r="AR1" t="s">
-        <v>379</v>
-      </c>
-      <c r="AS1" t="s">
-        <v>380</v>
-      </c>
-      <c r="AT1" t="s">
-        <v>381</v>
-      </c>
-      <c r="AU1" t="s">
-        <v>382</v>
-      </c>
       <c r="AV1" t="s">
+        <v>385</v>
+      </c>
+      <c r="AW1" t="s">
+        <v>387</v>
+      </c>
+      <c r="AX1" t="s">
+        <v>386</v>
+      </c>
+      <c r="AY1" t="s">
+        <v>388</v>
+      </c>
+      <c r="AZ1" t="s">
         <v>383</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="BA1" t="s">
         <v>384</v>
       </c>
-      <c r="AX1" t="s">
-        <v>385</v>
-      </c>
-      <c r="AY1" t="s">
-        <v>386</v>
-      </c>
-      <c r="AZ1" t="s">
-        <v>387</v>
-      </c>
-      <c r="BA1" t="s">
-        <v>388</v>
-      </c>
       <c r="BB1" t="s">
+        <v>391</v>
+      </c>
+      <c r="BC1" t="s">
+        <v>393</v>
+      </c>
+      <c r="BD1" t="s">
+        <v>392</v>
+      </c>
+      <c r="BE1" t="s">
+        <v>424</v>
+      </c>
+      <c r="BF1" t="s">
         <v>389</v>
       </c>
-      <c r="BC1" t="s">
+      <c r="BG1" t="s">
         <v>390</v>
       </c>
-      <c r="BD1" t="s">
-        <v>391</v>
-      </c>
-      <c r="BE1" t="s">
-        <v>391</v>
-      </c>
-      <c r="BF1" t="s">
-        <v>392</v>
-      </c>
-      <c r="BG1" t="s">
-        <v>393</v>
-      </c>
       <c r="BH1" t="s">
+        <v>397</v>
+      </c>
+      <c r="BI1" t="s">
+        <v>399</v>
+      </c>
+      <c r="BJ1" t="s">
+        <v>398</v>
+      </c>
+      <c r="BK1" t="s">
         <v>394</v>
       </c>
-      <c r="BI1" t="s">
+      <c r="BL1" t="s">
         <v>395</v>
       </c>
-      <c r="BJ1" t="s">
+      <c r="BM1" t="s">
         <v>396</v>
       </c>
-      <c r="BK1" t="s">
-        <v>397</v>
-      </c>
-      <c r="BL1" t="s">
-        <v>398</v>
-      </c>
-      <c r="BM1" t="s">
-        <v>399</v>
-      </c>
       <c r="BN1" t="s">
+        <v>403</v>
+      </c>
+      <c r="BO1" t="s">
+        <v>425</v>
+      </c>
+      <c r="BP1" t="s">
+        <v>404</v>
+      </c>
+      <c r="BQ1" t="s">
         <v>400</v>
       </c>
-      <c r="BO1" t="s">
+      <c r="BR1" t="s">
         <v>401</v>
       </c>
-      <c r="BP1" t="s">
+      <c r="BS1" t="s">
         <v>402</v>
       </c>
-      <c r="BQ1" t="s">
-        <v>403</v>
-      </c>
-      <c r="BR1" t="s">
-        <v>403</v>
-      </c>
-      <c r="BS1" t="s">
-        <v>404</v>
-      </c>
       <c r="BT1" t="s">
+        <v>409</v>
+      </c>
+      <c r="BU1" t="s">
         <v>405</v>
       </c>
-      <c r="BU1" t="s">
+      <c r="BV1" t="s">
+        <v>410</v>
+      </c>
+      <c r="BW1" t="s">
         <v>406</v>
       </c>
-      <c r="BV1" t="s">
+      <c r="BX1" t="s">
         <v>407</v>
       </c>
-      <c r="BW1" t="s">
+      <c r="BY1" t="s">
         <v>408</v>
       </c>
-      <c r="BX1" t="s">
-        <v>409</v>
-      </c>
-      <c r="BY1" t="s">
-        <v>410</v>
-      </c>
       <c r="BZ1" t="s">
+        <v>415</v>
+      </c>
+      <c r="CA1" t="s">
         <v>411</v>
       </c>
-      <c r="CA1" t="s">
+      <c r="CB1" t="s">
+        <v>426</v>
+      </c>
+      <c r="CC1" t="s">
         <v>412</v>
       </c>
-      <c r="CB1" t="s">
+      <c r="CD1" t="s">
         <v>413</v>
       </c>
-      <c r="CC1" t="s">
+      <c r="CE1" t="s">
         <v>414</v>
       </c>
-      <c r="CD1" t="s">
-        <v>415</v>
-      </c>
-      <c r="CE1" t="s">
-        <v>415</v>
-      </c>
       <c r="CF1" t="s">
-        <v>416</v>
+        <v>421</v>
       </c>
       <c r="CG1" t="s">
         <v>417</v>
       </c>
       <c r="CH1" t="s">
+        <v>416</v>
+      </c>
+      <c r="CI1" t="s">
         <v>418</v>
       </c>
-      <c r="CI1" t="s">
+      <c r="CJ1" t="s">
         <v>419</v>
       </c>
-      <c r="CJ1" t="s">
+      <c r="CK1" t="s">
         <v>420</v>
-      </c>
-      <c r="CK1" t="s">
-        <v>421</v>
       </c>
     </row>
     <row r="2" spans="1:89" x14ac:dyDescent="0.15">

</xml_diff>